<commit_message>
actually finish wk1 now that poster page is up. and add more content to index page
</commit_message>
<xml_diff>
--- a/schedule_615_test.xlsx
+++ b/schedule_615_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C65F3E4-824A-498E-BEB6-0F8E8CF9EE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723C25AF-F3D9-4E3F-91C5-A5D6489DAB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29370" yWindow="1590" windowWidth="27840" windowHeight="12330" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -451,9 +451,6 @@
     <t>lecture</t>
   </si>
   <si>
-    <t>Project Introduction</t>
-  </si>
-  <si>
     <t>lec01-data-arch</t>
   </si>
   <si>
@@ -467,6 +464,9 @@
 Spreadsheets are a common method of recording data
 Codebooks are an essential piece in learning about the data
 There is a difference between human readable and computer readable data formats</t>
+  </si>
+  <si>
+    <t>Project Stage 1: Choosing your topic</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1332,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E4" sqref="E4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1370,7 +1370,7 @@
         <v>118</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H1" s="34" t="s">
         <v>129</v>
@@ -1408,7 +1408,7 @@
         <v>119</v>
       </c>
       <c r="G2" s="46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H2" s="41" t="s">
         <v>121</v>
@@ -1443,10 +1443,10 @@
         <v>120</v>
       </c>
       <c r="G3" s="46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I3" s="41" t="s">
         <v>98</v>
@@ -1467,10 +1467,10 @@
       <c r="D4" s="27">
         <v>1.3</v>
       </c>
-      <c r="E4" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="F4" s="46" t="s">
+      <c r="E4" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="41" t="s">
         <v>125</v>
       </c>
       <c r="G4" s="46"/>

</xml_diff>